<commit_message>
Aryl Halide Results++: 200 epochs and LR 0.0001
</commit_message>
<xml_diff>
--- a/yield_prediction/results/graph_descriptors/WL_gnn/out_of_sample/aryl_halide/ranking_test1/results.xlsx
+++ b/yield_prediction/results/graph_descriptors/WL_gnn/out_of_sample/aryl_halide/ranking_test1/results.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3573,6 +3573,1038 @@
         <v>16.618</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>5</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>251.051</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="I74" t="n">
+        <v>15.343</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="K74" t="n">
+        <v>15.087</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>4</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>268.523</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.681</v>
+      </c>
+      <c r="I75" t="n">
+        <v>15.671</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="K75" t="n">
+        <v>15.663</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>4</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>262.868</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="I76" t="n">
+        <v>15.706</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="K76" t="n">
+        <v>15.846</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>5</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>257.144</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="I77" t="n">
+        <v>15.468</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.591</v>
+      </c>
+      <c r="K77" t="n">
+        <v>14.761</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>5</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>252.722</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="I78" t="n">
+        <v>15.341</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.553</v>
+      </c>
+      <c r="K78" t="n">
+        <v>15.436</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>4</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>268.598</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="I79" t="n">
+        <v>15.685</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="K79" t="n">
+        <v>15.984</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>3</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>251.058</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="I80" t="n">
+        <v>15.474</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.584</v>
+      </c>
+      <c r="K80" t="n">
+        <v>14.898</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>5</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>273.913</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I81" t="n">
+        <v>15.936</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="K81" t="n">
+        <v>15.817</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>4</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>246.164</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0.716</v>
+      </c>
+      <c r="I82" t="n">
+        <v>14.78</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="K82" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>5</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>185.978</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0.779</v>
+      </c>
+      <c r="I83" t="n">
+        <v>13.077</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.639</v>
+      </c>
+      <c r="K83" t="n">
+        <v>13.818</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>4</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>257.569</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0.6919999999999999</v>
+      </c>
+      <c r="I84" t="n">
+        <v>15.465</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.521</v>
+      </c>
+      <c r="K84" t="n">
+        <v>16.086</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>5</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>304.533</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.634</v>
+      </c>
+      <c r="I85" t="n">
+        <v>16.967</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="K85" t="n">
+        <v>18.869</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>4</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>303.137</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.624</v>
+      </c>
+      <c r="I86" t="n">
+        <v>17.04</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.417</v>
+      </c>
+      <c r="K86" t="n">
+        <v>17.618</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>5</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>299.845</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="I87" t="n">
+        <v>16.857</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="K87" t="n">
+        <v>17.548</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>4</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>327.618</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="I88" t="n">
+        <v>17.659</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0.319</v>
+      </c>
+      <c r="K88" t="n">
+        <v>19.115</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>3</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>262.354</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.674</v>
+      </c>
+      <c r="I89" t="n">
+        <v>15.886</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0.518</v>
+      </c>
+      <c r="K89" t="n">
+        <v>15.947</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>3</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>270.111</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="I90" t="n">
+        <v>15.986</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0.496</v>
+      </c>
+      <c r="K90" t="n">
+        <v>16.404</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>5</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>254.068</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.694</v>
+      </c>
+      <c r="I91" t="n">
+        <v>15.429</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="K91" t="n">
+        <v>16.465</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>5</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>307.384</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.617</v>
+      </c>
+      <c r="I92" t="n">
+        <v>17.267</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="K92" t="n">
+        <v>18.218</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>4</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>189.158</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.777</v>
+      </c>
+      <c r="I93" t="n">
+        <v>13.117</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="K93" t="n">
+        <v>13.637</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>4</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>241.99</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.731</v>
+      </c>
+      <c r="I94" t="n">
+        <v>14.499</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.458</v>
+      </c>
+      <c r="K94" t="n">
+        <v>17.051</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>5</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>228.132</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.723</v>
+      </c>
+      <c r="I95" t="n">
+        <v>14.632</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.554</v>
+      </c>
+      <c r="K95" t="n">
+        <v>15.314</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>4</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>281.859</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I96" t="n">
+        <v>16.002</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.501</v>
+      </c>
+      <c r="K96" t="n">
+        <v>16.419</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>aryl_halide_200epochs</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>ranking_test1</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>4</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>352.875</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.5590000000000001</v>
+      </c>
+      <c r="I97" t="n">
+        <v>18.54</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0.327</v>
+      </c>
+      <c r="K97" t="n">
+        <v>18.76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>